<commit_message>
Node Rev.2:   DC-DC-Converter replaced by one with a smaller footprint
</commit_message>
<xml_diff>
--- a/Wiring.xlsx
+++ b/Wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Wiring the wagons</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>https://www.amazon.de/gp/product/B07NQCB92N/ref=ox_sc_act_title_1?smid=A2PNNIYOUQZRLT&amp;psc=1</t>
+  </si>
+  <si>
+    <t>max. animations at the same time</t>
+  </si>
+  <si>
+    <t>DC converter output</t>
+  </si>
+  <si>
+    <t>max. dc converter output current</t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
     <numFmt numFmtId="164" formatCode="0.00\ &quot;m&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;A&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0\ &quot;V&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.00\ &quot;Ohm&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;Ohm&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -152,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -255,15 +264,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>135802</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>344032</xdr:rowOff>
+      <xdr:colOff>36214</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>172016</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>407405</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>108642</xdr:rowOff>
+      <xdr:colOff>307817</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>316872</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -272,7 +281,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3431263" y="1792586"/>
+          <a:off x="3331675" y="2933323"/>
           <a:ext cx="2589291" cy="1412341"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -315,7 +324,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-DE" sz="1100"/>
-            <a:t>Feel freuu to adopt these values as</a:t>
+            <a:t>Feel free to adopt these values as</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" baseline="0"/>
@@ -633,7 +642,7 @@
   <dimension ref="B2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -736,6 +745,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+    </row>
     <row r="18" spans="2:3" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>8</v>
@@ -745,6 +762,14 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="19" spans="2:3" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
     <row r="20" spans="2:3" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>9</v>
@@ -770,6 +795,15 @@
       <c r="C23">
         <f>SQRT(4*C22/PI())</f>
         <v>0.44451674467406854</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <f>ROUNDDOWN(C9/ (C17*C19/C14),0)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>